<commit_message>
Updated Report for ESP-IDF setup
</commit_message>
<xml_diff>
--- a/Documentation/Reports/TimeReport_CarterKreis.xlsx
+++ b/Documentation/Reports/TimeReport_CarterKreis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\plant-partner\Documentation\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559D6619-EF74-4006-85BB-A39CCA7677E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760B25F4-BAD6-45A5-B00E-BFAC3A00C294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Name:</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Check-in 3: Met with group &amp; Tyler. Planned out pre-alpha build documentation, materials list, and basic codebase structure. I will be working on PCB Design and physical materials for prototypes</t>
+  </si>
+  <si>
+    <t>Pre-Alpha Build</t>
+  </si>
+  <si>
+    <t>Researched and begun setup of ESP-IDF through its VS Code extension</t>
   </si>
 </sst>
 </file>
@@ -540,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,7 +573,7 @@
       </c>
       <c r="E1" s="4">
         <f>SUM(E4:E199)</f>
-        <v>0.23611111111111127</v>
+        <v>0.25694444444444464</v>
       </c>
       <c r="F1" s="5"/>
     </row>
@@ -605,7 +611,7 @@
         <v>0.61041666666666672</v>
       </c>
       <c r="E4" s="9">
-        <f>D4-C4</f>
+        <f t="shared" ref="E4:E9" si="0">D4-C4</f>
         <v>0.14027777777777783</v>
       </c>
       <c r="F4" s="10" t="s">
@@ -626,7 +632,7 @@
         <v>0.64722222222222225</v>
       </c>
       <c r="E5" s="9">
-        <f>D5-C5</f>
+        <f t="shared" si="0"/>
         <v>2.2222222222222254E-2</v>
       </c>
       <c r="F5" s="10" t="s">
@@ -647,7 +653,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E6" s="14">
-        <f>D6-C6</f>
+        <f t="shared" si="0"/>
         <v>2.9861111111111116E-2</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -668,7 +674,7 @@
         <v>0.49375000000000002</v>
       </c>
       <c r="E7" s="9">
-        <f>D7-C7</f>
+        <f t="shared" si="0"/>
         <v>2.1527777777777812E-2</v>
       </c>
       <c r="F7" s="10" t="s">
@@ -689,7 +695,7 @@
         <v>0.64722222222222225</v>
       </c>
       <c r="E8" s="9">
-        <f>D8-C8</f>
+        <f t="shared" si="0"/>
         <v>2.2222222222222254E-2</v>
       </c>
       <c r="F8" s="10" t="s">
@@ -697,15 +703,25 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="6">
+        <v>45950</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.90625</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.92708333333333337</v>
+      </c>
       <c r="E9" s="9">
-        <f>D9-C9</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="10"/>
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
@@ -713,7 +729,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="9">
-        <f t="shared" ref="E10:E68" si="0">D10-C10</f>
+        <f t="shared" ref="E10:E68" si="1">D10-C10</f>
         <v>0</v>
       </c>
       <c r="F10" s="10"/>
@@ -724,7 +740,7 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F11" s="10"/>
@@ -735,7 +751,7 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F12" s="10"/>
@@ -746,7 +762,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F13" s="10"/>
@@ -757,7 +773,7 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F14" s="10"/>
@@ -768,7 +784,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F15" s="10"/>
@@ -779,7 +795,7 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F16" s="10"/>
@@ -790,7 +806,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F17" s="10"/>
@@ -801,7 +817,7 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F18" s="10"/>
@@ -812,7 +828,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F19" s="10"/>
@@ -823,7 +839,7 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F20" s="10"/>
@@ -834,7 +850,7 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F21" s="10"/>
@@ -845,7 +861,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F22" s="10"/>
@@ -856,7 +872,7 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F23" s="10"/>
@@ -867,7 +883,7 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F24" s="10"/>
@@ -878,7 +894,7 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F25" s="10"/>
@@ -889,7 +905,7 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F26" s="10"/>
@@ -900,7 +916,7 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F27" s="10"/>
@@ -911,7 +927,7 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F28" s="10"/>
@@ -922,7 +938,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F29" s="10"/>
@@ -933,7 +949,7 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F30" s="10"/>
@@ -944,7 +960,7 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F31" s="10"/>
@@ -955,7 +971,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F32" s="10"/>
@@ -966,7 +982,7 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F33" s="10"/>
@@ -977,7 +993,7 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F34" s="10"/>
@@ -988,7 +1004,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F35" s="10"/>
@@ -999,7 +1015,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F36" s="10"/>
@@ -1010,7 +1026,7 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F37" s="10"/>
@@ -1021,7 +1037,7 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F38" s="10"/>
@@ -1032,7 +1048,7 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F39" s="10"/>
@@ -1043,7 +1059,7 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F40" s="10"/>
@@ -1054,7 +1070,7 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F41" s="10"/>
@@ -1065,7 +1081,7 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F42" s="10"/>
@@ -1076,7 +1092,7 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F43" s="10"/>
@@ -1087,7 +1103,7 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F44" s="10"/>
@@ -1098,7 +1114,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F45" s="10"/>
@@ -1109,7 +1125,7 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F46" s="10"/>
@@ -1120,7 +1136,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F47" s="10"/>
@@ -1131,7 +1147,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F48" s="10"/>
@@ -1142,7 +1158,7 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F49" s="10"/>
@@ -1153,7 +1169,7 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F50" s="10"/>
@@ -1164,7 +1180,7 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F51" s="10"/>
@@ -1175,7 +1191,7 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F52" s="10"/>
@@ -1186,7 +1202,7 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F53" s="10"/>
@@ -1197,7 +1213,7 @@
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F54" s="10"/>
@@ -1208,7 +1224,7 @@
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F55" s="10"/>
@@ -1219,7 +1235,7 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F56" s="10"/>
@@ -1230,7 +1246,7 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F57" s="10"/>
@@ -1241,7 +1257,7 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F58" s="10"/>
@@ -1252,7 +1268,7 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F59" s="10"/>
@@ -1263,7 +1279,7 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F60" s="10"/>
@@ -1274,7 +1290,7 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F61" s="10"/>
@@ -1285,7 +1301,7 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F62" s="10"/>
@@ -1296,7 +1312,7 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F63" s="10"/>
@@ -1307,7 +1323,7 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F64" s="10"/>
@@ -1318,7 +1334,7 @@
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F65" s="10"/>
@@ -1329,7 +1345,7 @@
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F66" s="10"/>
@@ -1340,7 +1356,7 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F67" s="10"/>
@@ -1351,7 +1367,7 @@
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F68" s="10"/>
@@ -1362,7 +1378,7 @@
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="9">
-        <f t="shared" ref="E69:E132" si="1">D69-C69</f>
+        <f t="shared" ref="E69:E132" si="2">D69-C69</f>
         <v>0</v>
       </c>
       <c r="F69" s="10"/>
@@ -1373,7 +1389,7 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F70" s="10"/>
@@ -1384,7 +1400,7 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F71" s="10"/>
@@ -1395,7 +1411,7 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F72" s="10"/>
@@ -1406,7 +1422,7 @@
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F73" s="10"/>
@@ -1417,7 +1433,7 @@
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F74" s="10"/>
@@ -1428,7 +1444,7 @@
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F75" s="10"/>
@@ -1439,7 +1455,7 @@
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F76" s="10"/>
@@ -1450,7 +1466,7 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F77" s="10"/>
@@ -1461,7 +1477,7 @@
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F78" s="10"/>
@@ -1472,7 +1488,7 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F79" s="10"/>
@@ -1483,7 +1499,7 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F80" s="10"/>
@@ -1494,7 +1510,7 @@
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F81" s="10"/>
@@ -1505,7 +1521,7 @@
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F82" s="10"/>
@@ -1516,7 +1532,7 @@
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F83" s="10"/>
@@ -1527,7 +1543,7 @@
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F84" s="10"/>
@@ -1538,7 +1554,7 @@
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F85" s="10"/>
@@ -1549,7 +1565,7 @@
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F86" s="10"/>
@@ -1560,7 +1576,7 @@
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F87" s="10"/>
@@ -1571,7 +1587,7 @@
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F88" s="10"/>
@@ -1582,7 +1598,7 @@
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F89" s="10"/>
@@ -1593,7 +1609,7 @@
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F90" s="10"/>
@@ -1604,7 +1620,7 @@
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
       <c r="E91" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F91" s="10"/>
@@ -1615,7 +1631,7 @@
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
       <c r="E92" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F92" s="10"/>
@@ -1626,7 +1642,7 @@
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
       <c r="E93" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F93" s="10"/>
@@ -1637,7 +1653,7 @@
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
       <c r="E94" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F94" s="10"/>
@@ -1648,7 +1664,7 @@
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
       <c r="E95" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F95" s="10"/>
@@ -1659,7 +1675,7 @@
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
       <c r="E96" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F96" s="10"/>
@@ -1670,7 +1686,7 @@
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F97" s="10"/>
@@ -1681,7 +1697,7 @@
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
       <c r="E98" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F98" s="10"/>
@@ -1692,7 +1708,7 @@
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
       <c r="E99" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F99" s="10"/>
@@ -1703,7 +1719,7 @@
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
       <c r="E100" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F100" s="10"/>
@@ -1714,7 +1730,7 @@
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
       <c r="E101" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F101" s="10"/>
@@ -1725,7 +1741,7 @@
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
       <c r="E102" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F102" s="10"/>
@@ -1736,7 +1752,7 @@
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F103" s="10"/>
@@ -1747,7 +1763,7 @@
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F104" s="10"/>
@@ -1758,7 +1774,7 @@
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F105" s="10"/>
@@ -1769,7 +1785,7 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F106" s="10"/>
@@ -1780,7 +1796,7 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F107" s="10"/>
@@ -1791,7 +1807,7 @@
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F108" s="10"/>
@@ -1802,7 +1818,7 @@
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F109" s="10"/>
@@ -1813,7 +1829,7 @@
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F110" s="10"/>
@@ -1824,7 +1840,7 @@
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F111" s="10"/>
@@ -1835,7 +1851,7 @@
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F112" s="10"/>
@@ -1846,7 +1862,7 @@
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F113" s="10"/>
@@ -1857,7 +1873,7 @@
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F114" s="10"/>
@@ -1868,7 +1884,7 @@
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F115" s="10"/>
@@ -1879,7 +1895,7 @@
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F116" s="10"/>
@@ -1890,7 +1906,7 @@
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F117" s="10"/>
@@ -1901,7 +1917,7 @@
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F118" s="10"/>
@@ -1912,7 +1928,7 @@
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F119" s="10"/>
@@ -1923,7 +1939,7 @@
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F120" s="10"/>
@@ -1934,7 +1950,7 @@
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F121" s="10"/>
@@ -1945,7 +1961,7 @@
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F122" s="10"/>
@@ -1956,7 +1972,7 @@
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F123" s="10"/>
@@ -1967,7 +1983,7 @@
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F124" s="10"/>
@@ -1978,7 +1994,7 @@
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F125" s="10"/>
@@ -1989,7 +2005,7 @@
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F126" s="10"/>
@@ -2000,7 +2016,7 @@
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F127" s="10"/>
@@ -2011,7 +2027,7 @@
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F128" s="10"/>
@@ -2022,7 +2038,7 @@
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
       <c r="E129" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F129" s="10"/>
@@ -2033,7 +2049,7 @@
       <c r="C130" s="7"/>
       <c r="D130" s="7"/>
       <c r="E130" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F130" s="10"/>
@@ -2044,7 +2060,7 @@
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F131" s="10"/>
@@ -2055,7 +2071,7 @@
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F132" s="10"/>
@@ -2066,7 +2082,7 @@
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="9">
-        <f t="shared" ref="E133:E196" si="2">D133-C133</f>
+        <f t="shared" ref="E133:E196" si="3">D133-C133</f>
         <v>0</v>
       </c>
       <c r="F133" s="10"/>
@@ -2077,7 +2093,7 @@
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
       <c r="E134" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F134" s="10"/>
@@ -2088,7 +2104,7 @@
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
       <c r="E135" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F135" s="10"/>
@@ -2099,7 +2115,7 @@
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
       <c r="E136" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F136" s="10"/>
@@ -2110,7 +2126,7 @@
       <c r="C137" s="7"/>
       <c r="D137" s="7"/>
       <c r="E137" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F137" s="10"/>
@@ -2121,7 +2137,7 @@
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
       <c r="E138" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F138" s="10"/>
@@ -2132,7 +2148,7 @@
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
       <c r="E139" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F139" s="10"/>
@@ -2143,7 +2159,7 @@
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
       <c r="E140" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F140" s="10"/>
@@ -2154,7 +2170,7 @@
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
       <c r="E141" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F141" s="10"/>
@@ -2165,7 +2181,7 @@
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
       <c r="E142" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F142" s="10"/>
@@ -2176,7 +2192,7 @@
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
       <c r="E143" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F143" s="10"/>
@@ -2187,7 +2203,7 @@
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
       <c r="E144" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F144" s="10"/>
@@ -2198,7 +2214,7 @@
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
       <c r="E145" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F145" s="10"/>
@@ -2209,7 +2225,7 @@
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
       <c r="E146" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F146" s="10"/>
@@ -2220,7 +2236,7 @@
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
       <c r="E147" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F147" s="10"/>
@@ -2231,7 +2247,7 @@
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
       <c r="E148" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F148" s="10"/>
@@ -2242,7 +2258,7 @@
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
       <c r="E149" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F149" s="10"/>
@@ -2253,7 +2269,7 @@
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
       <c r="E150" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F150" s="10"/>
@@ -2264,7 +2280,7 @@
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
       <c r="E151" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F151" s="10"/>
@@ -2275,7 +2291,7 @@
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
       <c r="E152" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F152" s="10"/>
@@ -2286,7 +2302,7 @@
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
       <c r="E153" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F153" s="10"/>
@@ -2297,7 +2313,7 @@
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F154" s="10"/>
@@ -2308,7 +2324,7 @@
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
       <c r="E155" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F155" s="10"/>
@@ -2319,7 +2335,7 @@
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
       <c r="E156" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F156" s="10"/>
@@ -2330,7 +2346,7 @@
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
       <c r="E157" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F157" s="10"/>
@@ -2341,7 +2357,7 @@
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
       <c r="E158" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F158" s="10"/>
@@ -2352,7 +2368,7 @@
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
       <c r="E159" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F159" s="10"/>
@@ -2363,7 +2379,7 @@
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
       <c r="E160" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F160" s="10"/>
@@ -2374,7 +2390,7 @@
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
       <c r="E161" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F161" s="10"/>
@@ -2385,7 +2401,7 @@
       <c r="C162" s="7"/>
       <c r="D162" s="7"/>
       <c r="E162" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F162" s="10"/>
@@ -2396,7 +2412,7 @@
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
       <c r="E163" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F163" s="10"/>
@@ -2407,7 +2423,7 @@
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F164" s="10"/>
@@ -2418,7 +2434,7 @@
       <c r="C165" s="7"/>
       <c r="D165" s="7"/>
       <c r="E165" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F165" s="10"/>
@@ -2429,7 +2445,7 @@
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
       <c r="E166" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F166" s="10"/>
@@ -2440,7 +2456,7 @@
       <c r="C167" s="7"/>
       <c r="D167" s="7"/>
       <c r="E167" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F167" s="10"/>
@@ -2451,7 +2467,7 @@
       <c r="C168" s="7"/>
       <c r="D168" s="7"/>
       <c r="E168" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F168" s="10"/>
@@ -2462,7 +2478,7 @@
       <c r="C169" s="7"/>
       <c r="D169" s="7"/>
       <c r="E169" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F169" s="10"/>
@@ -2473,7 +2489,7 @@
       <c r="C170" s="7"/>
       <c r="D170" s="7"/>
       <c r="E170" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F170" s="10"/>
@@ -2484,7 +2500,7 @@
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
       <c r="E171" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F171" s="10"/>
@@ -2495,7 +2511,7 @@
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
       <c r="E172" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F172" s="10"/>
@@ -2506,7 +2522,7 @@
       <c r="C173" s="7"/>
       <c r="D173" s="7"/>
       <c r="E173" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F173" s="10"/>
@@ -2517,7 +2533,7 @@
       <c r="C174" s="7"/>
       <c r="D174" s="7"/>
       <c r="E174" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F174" s="10"/>
@@ -2528,7 +2544,7 @@
       <c r="C175" s="7"/>
       <c r="D175" s="7"/>
       <c r="E175" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F175" s="10"/>
@@ -2539,7 +2555,7 @@
       <c r="C176" s="7"/>
       <c r="D176" s="7"/>
       <c r="E176" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F176" s="10"/>
@@ -2550,7 +2566,7 @@
       <c r="C177" s="7"/>
       <c r="D177" s="7"/>
       <c r="E177" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F177" s="10"/>
@@ -2561,7 +2577,7 @@
       <c r="C178" s="7"/>
       <c r="D178" s="7"/>
       <c r="E178" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F178" s="10"/>
@@ -2572,7 +2588,7 @@
       <c r="C179" s="7"/>
       <c r="D179" s="7"/>
       <c r="E179" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F179" s="10"/>
@@ -2583,7 +2599,7 @@
       <c r="C180" s="7"/>
       <c r="D180" s="7"/>
       <c r="E180" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F180" s="10"/>
@@ -2594,7 +2610,7 @@
       <c r="C181" s="7"/>
       <c r="D181" s="7"/>
       <c r="E181" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F181" s="10"/>
@@ -2605,7 +2621,7 @@
       <c r="C182" s="7"/>
       <c r="D182" s="7"/>
       <c r="E182" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F182" s="10"/>
@@ -2616,7 +2632,7 @@
       <c r="C183" s="7"/>
       <c r="D183" s="7"/>
       <c r="E183" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F183" s="10"/>
@@ -2627,7 +2643,7 @@
       <c r="C184" s="7"/>
       <c r="D184" s="7"/>
       <c r="E184" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F184" s="10"/>
@@ -2638,7 +2654,7 @@
       <c r="C185" s="7"/>
       <c r="D185" s="7"/>
       <c r="E185" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F185" s="10"/>
@@ -2649,7 +2665,7 @@
       <c r="C186" s="7"/>
       <c r="D186" s="7"/>
       <c r="E186" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F186" s="10"/>
@@ -2660,7 +2676,7 @@
       <c r="C187" s="7"/>
       <c r="D187" s="7"/>
       <c r="E187" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F187" s="10"/>
@@ -2671,7 +2687,7 @@
       <c r="C188" s="7"/>
       <c r="D188" s="7"/>
       <c r="E188" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F188" s="10"/>
@@ -2682,7 +2698,7 @@
       <c r="C189" s="7"/>
       <c r="D189" s="7"/>
       <c r="E189" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F189" s="10"/>
@@ -2693,7 +2709,7 @@
       <c r="C190" s="7"/>
       <c r="D190" s="7"/>
       <c r="E190" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F190" s="10"/>
@@ -2704,7 +2720,7 @@
       <c r="C191" s="7"/>
       <c r="D191" s="7"/>
       <c r="E191" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F191" s="10"/>
@@ -2715,7 +2731,7 @@
       <c r="C192" s="7"/>
       <c r="D192" s="7"/>
       <c r="E192" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F192" s="10"/>
@@ -2726,7 +2742,7 @@
       <c r="C193" s="7"/>
       <c r="D193" s="7"/>
       <c r="E193" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F193" s="10"/>
@@ -2737,7 +2753,7 @@
       <c r="C194" s="7"/>
       <c r="D194" s="7"/>
       <c r="E194" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F194" s="10"/>
@@ -2748,7 +2764,7 @@
       <c r="C195" s="7"/>
       <c r="D195" s="7"/>
       <c r="E195" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F195" s="10"/>
@@ -2759,7 +2775,7 @@
       <c r="C196" s="7"/>
       <c r="D196" s="7"/>
       <c r="E196" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F196" s="10"/>
@@ -2770,7 +2786,7 @@
       <c r="C197" s="7"/>
       <c r="D197" s="7"/>
       <c r="E197" s="9">
-        <f t="shared" ref="E197:E199" si="3">D197-C197</f>
+        <f t="shared" ref="E197:E199" si="4">D197-C197</f>
         <v>0</v>
       </c>
       <c r="F197" s="10"/>
@@ -2781,7 +2797,7 @@
       <c r="C198" s="7"/>
       <c r="D198" s="7"/>
       <c r="E198" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F198" s="10"/>
@@ -2792,7 +2808,7 @@
       <c r="C199" s="7"/>
       <c r="D199" s="7"/>
       <c r="E199" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F199" s="10"/>

</xml_diff>

<commit_message>
Added my horrendous timesheet
</commit_message>
<xml_diff>
--- a/Documentation/Reports/TimeReport_CarterKreis.xlsx
+++ b/Documentation/Reports/TimeReport_CarterKreis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\plant-partner\Documentation\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760B25F4-BAD6-45A5-B00E-BFAC3A00C294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731340B2-2179-4E22-A202-F66FD76CCDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
+    <workbookView xWindow="5760" yWindow="2436" windowWidth="17280" windowHeight="8964" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Name:</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Researched and begun setup of ESP-IDF through its VS Code extension</t>
+  </si>
+  <si>
+    <t>Setup ESP-IDF extension in VS Code. Attempted Hello World example code but my laptop is not detecting ESP32 as a COM Port. We also continued to plan Pre-Alpha Build goal</t>
+  </si>
+  <si>
+    <t>Repeated issues with recursively cloning the submodule esp-idf. Cloning into the submodule itself took 10-12 minutes and the first two times some of the directories failed to clone on time.</t>
   </si>
 </sst>
 </file>
@@ -169,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -201,6 +207,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -546,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,7 +582,7 @@
       </c>
       <c r="E1" s="4">
         <f>SUM(E4:E199)</f>
-        <v>0.25694444444444464</v>
+        <v>0.39444444444444465</v>
       </c>
       <c r="F1" s="5"/>
     </row>
@@ -724,26 +733,46 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="A10" s="6">
+        <v>45954</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="15">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0.1701388888888889</v>
+      </c>
       <c r="E10" s="9">
         <f t="shared" ref="E10:E68" si="1">D10-C10</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="10"/>
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="A11" s="6">
+        <v>45954</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="15">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="D11" s="15">
+        <v>0.37361111111111112</v>
+      </c>
       <c r="E11" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="10"/>
+        <v>7.1527777777777801E-2</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>

</xml_diff>